<commit_message>
formatted legend and title
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryhirsch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryhirsch/Henry/Git/mpp_capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F743EBE-E82F-6B40-ACD9-C134B5E747D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E700060-35A6-EC46-BD6A-5C781D7A7712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="500" windowWidth="28040" windowHeight="17500" xr2:uid="{ED54E7AF-918D-6942-8BE0-8995CE7F89AD}"/>
   </bookViews>
@@ -289,7 +289,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,9 +626,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912BAEF0-4E54-054D-8610-5197CA3567BF}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,7 +646,7 @@
     <col min="12" max="12" width="13.5" customWidth="1"/>
     <col min="13" max="13" width="16.5" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -693,7 +693,7 @@
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="P1" t="s">
@@ -743,10 +743,10 @@
       <c r="N2">
         <v>17</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <v>5945</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <v>9805</v>
       </c>
     </row>
@@ -793,10 +793,10 @@
       <c r="N3">
         <v>17</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>5336</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="1">
         <v>8348</v>
       </c>
     </row>
@@ -893,10 +893,10 @@
       <c r="N5">
         <v>26</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <v>7035</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="1">
         <v>12539</v>
       </c>
     </row>
@@ -943,10 +943,10 @@
       <c r="N6">
         <v>17</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <v>3654</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="1">
         <v>6145</v>
       </c>
     </row>
@@ -993,10 +993,10 @@
       <c r="N7">
         <v>19</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="1">
         <v>11475</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="1">
         <v>21697</v>
       </c>
     </row>
@@ -1043,10 +1043,10 @@
       <c r="N8">
         <v>10</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="1">
         <v>2075</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="1">
         <v>3510</v>
       </c>
     </row>
@@ -1093,10 +1093,10 @@
       <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="1">
         <v>247</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="1">
         <v>380</v>
       </c>
     </row>
@@ -1143,10 +1143,10 @@
       <c r="N10">
         <v>0</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="1">
         <v>607</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="1">
         <v>1011</v>
       </c>
     </row>
@@ -1193,10 +1193,10 @@
       <c r="N11">
         <v>71</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="1">
         <v>53525</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="1">
         <v>100893</v>
       </c>
     </row>
@@ -1243,10 +1243,10 @@
       <c r="N12">
         <v>46</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="1">
         <v>31010</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="1">
         <v>70700</v>
       </c>
     </row>
@@ -1293,10 +1293,10 @@
       <c r="N13">
         <v>146</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="1">
         <v>32953</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="1">
         <v>57473</v>
       </c>
     </row>
@@ -1328,10 +1328,10 @@
       <c r="N14">
         <v>4</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="1">
         <v>570</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="1">
         <v>891</v>
       </c>
     </row>
@@ -1378,10 +1378,10 @@
       <c r="N15">
         <v>4</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <v>522</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="1">
         <v>788</v>
       </c>
     </row>
@@ -1428,10 +1428,10 @@
       <c r="N16">
         <v>99</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="1">
         <v>17348</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="1">
         <v>24960</v>
       </c>
     </row>

</xml_diff>